<commit_message>
7/12 update CCFinder 100M
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="52">
   <si>
     <t>SourcerCC</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>19min49s</t>
+  </si>
+  <si>
+    <t>9h49min</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +767,9 @@
       <c r="B19" t="s">
         <v>34</v>
       </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
       <c r="D19" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
713 inserted MY record
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>SourcerCC</t>
   </si>
@@ -184,18 +184,53 @@
   </si>
   <si>
     <t>6min30s</t>
+  </si>
+  <si>
+    <t>MY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>59s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12min23s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -525,21 +560,21 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
+    <col min="4" max="4" width="13.75" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -557,7 +592,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -574,7 +609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>16</v>
       </c>
@@ -585,7 +620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1</v>
       </c>
@@ -596,7 +631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>4</v>
       </c>
@@ -607,7 +642,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -627,7 +662,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>8</v>
       </c>
@@ -644,7 +679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>16</v>
       </c>
@@ -661,7 +696,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>8</v>
       </c>
@@ -675,7 +710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>4</v>
       </c>
@@ -692,20 +727,22 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="1"/>
       <c r="H14" s="3" t="s">
         <v>28</v>
       </c>
@@ -720,94 +757,112 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
       </c>
       <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>49</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>47</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -822,7 +877,7 @@
       <c r="F22" s="2"/>
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -830,7 +885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -841,7 +896,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -852,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -863,7 +918,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -874,13 +929,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
7/18 Add python file
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -174,9 +174,6 @@
     <t>12min31s</t>
   </si>
   <si>
-    <t>6min30s</t>
-  </si>
-  <si>
     <t>MY</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -215,6 +212,9 @@
   </si>
   <si>
     <t>114282KB</t>
+  </si>
+  <si>
+    <t>7min29s</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,7 +647,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -735,10 +735,10 @@
         <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -765,7 +765,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -782,7 +782,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -799,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
@@ -816,13 +816,13 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>47</v>
@@ -833,13 +833,13 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E19" t="s">
         <v>45</v>
@@ -850,7 +850,7 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -870,7 +870,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>37</v>
@@ -917,7 +917,7 @@
         <v>13594</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -928,7 +928,7 @@
         <v>363761</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:13">

</xml_diff>